<commit_message>
typo(UX): Fixed a typo in JdT
</commit_message>
<xml_diff>
--- a/UX/T-P_ShootMeUp-ESR-JdT.xlsx
+++ b/UX/T-P_ShootMeUp-ESR-JdT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pg13qnw\Documents\GitHub\P_ShootMeUp-Eliott\UX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46968C0-3A4D-40D8-B2EA-32EDCF87C10D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FBE9C7D-5E2B-4F52-90B9-78A36A1BF5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -101,9 +101,6 @@
     <t>28.08.2024 au 1.11.2024</t>
   </si>
   <si>
-    <t>Création de la To-di list</t>
-  </si>
-  <si>
     <t>Création du premier persona</t>
   </si>
   <si>
@@ -129,6 +126,9 @@
   </si>
   <si>
     <t>Création du wireframe pour l'Editeur de niveaux</t>
+  </si>
+  <si>
+    <t>Création de la To-do list</t>
   </si>
 </sst>
 </file>
@@ -907,7 +907,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1035,7 +1035,7 @@
         <v>4</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="G7" s="37"/>
     </row>
@@ -1055,10 +1055,10 @@
         <v>2</v>
       </c>
       <c r="F8" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="46" t="s">
         <v>21</v>
-      </c>
-      <c r="G8" s="46" t="s">
-        <v>22</v>
       </c>
       <c r="M8" t="s">
         <v>2</v>
@@ -1086,7 +1086,7 @@
         <v>2</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G9" s="39"/>
       <c r="M9" t="s">
@@ -1115,10 +1115,10 @@
         <v>2</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G10" s="38" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M10" t="s">
         <v>3</v>
@@ -1146,7 +1146,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G11" s="39"/>
       <c r="M11" t="s">
@@ -1175,7 +1175,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G12" s="38"/>
       <c r="N12">
@@ -1201,7 +1201,7 @@
         <v>14</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G13" s="39"/>
       <c r="N13">
@@ -1227,7 +1227,7 @@
         <v>14</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G14" s="38"/>
       <c r="N14">
@@ -1255,7 +1255,7 @@
         <v>14</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G15" s="39"/>
       <c r="N15">
@@ -7535,6 +7535,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="34298955776df91f451dfdd912b0d80d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ed9741631eefaa61c396a6d47d02de0f" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -7729,27 +7749,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
+    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EE95A31-3997-42E6-AE6E-094AD61D4048}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7766,25 +7787,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
-    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>